<commit_message>
Amended OrderManagerUAT for Order Cancellation fixes
Fixed order cancelling method in OrderManagerUAT


Former-commit-id: 1d1af69188fc2740f107c022cd59b1c283ef882d
</commit_message>
<xml_diff>
--- a/IDB_Venue_Spreadsheet_Upload_Template.xlsx
+++ b/IDB_Venue_Spreadsheet_Upload_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evan.gerhard\Documents\GitHub\ION_jmkv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717EA18-7A7B-49C1-BE59-813C6377C1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EC7E5-1A9A-4A99-8AF4-AE5E40180E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="2475" windowWidth="43200" windowHeight="23445" xr2:uid="{50344497-20E7-49A2-B3FF-CA6FCCC847B8}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15945" xr2:uid="{50344497-20E7-49A2-B3FF-CA6FCCC847B8}"/>
   </bookViews>
   <sheets>
     <sheet name="BTEC" sheetId="1" r:id="rId1"/>
@@ -1317,1111 +1317,1113 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3871655563</v>
+        <v>#N/A Requesting Data...4112372333</v>
         <stp/>
         <stp>BDP|11120797096460563508</stp>
         <tr r="B5" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3929337451</v>
+        <v>#N/A Requesting Data...3920713558</v>
         <stp/>
         <stp>BDP|12115772685943837417</stp>
         <tr r="B53" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3903833859</v>
+        <v>#N/A Requesting Data...3996548624</v>
         <stp/>
         <stp>BDP|16130023195594825103</stp>
         <tr r="B52" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3124696753</v>
+        <v>#N/A Requesting Data...4190533236</v>
         <stp/>
         <stp>BDP|14140876098948982773</stp>
         <tr r="B164" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3346715748</v>
+        <v>#N/A Requesting Data...3650874627</v>
         <stp/>
         <stp>BDP|17194440374449295706</stp>
         <tr r="B245" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4112419780</v>
+        <v>#N/A Requesting Data...3722047424</v>
         <stp/>
         <stp>BDP|12444570206265452830</stp>
         <tr r="B198" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3419129126</v>
+        <v>#N/A Requesting Data...4278526559</v>
         <stp/>
         <stp>BDP|14561414696857327447</stp>
         <tr r="B195" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3383460065</v>
+        <v>#N/A Requesting Data...4107059570</v>
         <stp/>
         <stp>BDP|17368274805899333679</stp>
         <tr r="B41" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3798687709</v>
+        <v>#N/A Requesting Data...3814998288</v>
         <stp/>
         <stp>BDP|14188030864160565847</stp>
         <tr r="B228" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3136698345</v>
+        <v>#N/A Requesting Data...3766211912</v>
         <stp/>
         <stp>BDP|12779228401048551271</stp>
         <tr r="B180" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3340099291</v>
+        <v>#N/A Requesting Data...3719987084</v>
         <stp/>
         <stp>BDP|13795176484890258009</stp>
         <tr r="B290" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3314849313</v>
+        <v>#N/A Requesting Data...3667832099</v>
         <stp/>
         <stp>BDP|14313256312894930842</stp>
         <tr r="B380" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3357679618</v>
+        <v>#N/A Requesting Data...3660621102</v>
         <stp/>
         <stp>BDP|11879108908462873911</stp>
         <tr r="B316" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3374762143</v>
+        <v>#N/A Requesting Data...3555801776</v>
         <stp/>
         <stp>BDP|18207661802382908774</stp>
         <tr r="B147" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4070396938</v>
+        <v>#N/A Requesting Data...4122193984</v>
         <stp/>
         <stp>BDP|13888092839392179941</stp>
         <tr r="B273" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3011534705</v>
+        <v>#N/A Requesting Data...4032841931</v>
         <stp/>
         <stp>BDP|11472162187900259364</stp>
         <tr r="B150" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3215896144</v>
+        <v>#N/A Requesting Data...3786002216</v>
         <stp/>
         <stp>BDP|12690169002901567946</stp>
         <tr r="B58" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3275454318</v>
+        <v>#N/A Requesting Data...3939075834</v>
         <stp/>
         <stp>BDP|15607511490830764230</stp>
         <tr r="B241" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3810086044</v>
+        <v>#N/A Requesting Data...3776221205</v>
         <stp/>
         <stp>BDP|10776292290719472997</stp>
         <tr r="B373" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3844016440</v>
+        <v>#N/A Requesting Data...4228031013</v>
         <stp/>
         <stp>BDP|12868094716281060947</stp>
         <tr r="B76" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3962823643</v>
+        <v>#N/A Requesting Data...4053112334</v>
         <stp/>
         <stp>BDP|13996467519915725835</stp>
         <tr r="B63" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3766002055</v>
+        <v>#N/A Requesting Data...3885943057</v>
         <stp/>
         <stp>BDP|14272608407983507983</stp>
         <tr r="B187" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3543128302</v>
+        <v>#N/A Requesting Data...4256858814</v>
         <stp/>
         <stp>BDP|14072205783776289099</stp>
         <tr r="B179" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3220743480</v>
+        <v>#N/A Requesting Data...4098362786</v>
         <stp/>
         <stp>BDP|12472061657717168898</stp>
         <tr r="B265" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3318138217</v>
+        <v>#N/A Requesting Data...4050163441</v>
         <stp/>
         <stp>BDP|18079143709040957191</stp>
         <tr r="B385" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4074445244</v>
+        <v>#N/A Requesting Data...3660741475</v>
         <stp/>
         <stp>BDP|11151411471402432891</stp>
         <tr r="B143" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3623399850</v>
+        <v>#N/A Requesting Data...4208505847</v>
         <stp/>
         <stp>BDP|12341820728550243050</stp>
         <tr r="B272" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3141885319</v>
+        <v>#N/A Requesting Data...3872414456</v>
         <stp/>
         <stp>BDP|13855270601788982165</stp>
         <tr r="B12" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4087715399</v>
+        <v>#N/A Requesting Data...3615772759</v>
         <stp/>
         <stp>BDP|17703101299307860049</stp>
         <tr r="B112" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3731164178</v>
+        <v>#N/A Requesting Data...3824825864</v>
         <stp/>
         <stp>BDP|14373864853943426268</stp>
         <tr r="B91" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3479993344</v>
+        <v>#N/A Requesting Data...4204441414</v>
         <stp/>
         <stp>BDP|16049762620828654375</stp>
         <tr r="B246" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3282055824</v>
+        <v>#N/A Requesting Data...3744170179</v>
         <stp/>
         <stp>BDP|17173812374957355707</stp>
         <tr r="B358" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3715555503</v>
+        <v>#N/A Requesting Data...3567107397</v>
         <stp/>
         <stp>BDP|10499624187612106597</stp>
         <tr r="B32" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3736050515</v>
+        <v>#N/A Requesting Data...3495833588</v>
         <stp/>
         <stp>BDP|14960134837346266948</stp>
         <tr r="B182" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3642506583</v>
+        <v>#N/A Requesting Data...4079876900</v>
         <stp/>
         <stp>BDP|13132141980940966373</stp>
         <tr r="B188" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3177760232</v>
+        <v>#N/A Requesting Data...4234590579</v>
         <stp/>
         <stp>BDP|10312982465621375717</stp>
         <tr r="B170" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3387166001</v>
+        <v>#N/A Requesting Data...3636958398</v>
         <stp/>
         <stp>BDP|11316328163369802458</stp>
         <tr r="B352" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3155263470</v>
+        <v>#N/A Requesting Data...3620104113</v>
         <stp/>
         <stp>BDP|12495738690213939610</stp>
         <tr r="B348" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3753728422</v>
+        <v>#N/A Requesting Data...4269864532</v>
         <stp/>
         <stp>BDP|11193543237009773746</stp>
         <tr r="B336" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3551118972</v>
+        <v>#N/A Requesting Data...3540365682</v>
         <stp/>
         <stp>BDP|17455119081812061558</stp>
         <tr r="B26" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3518421795</v>
+        <v>#N/A Requesting Data...3707357209</v>
         <stp/>
         <stp>BDP|12080866041575484227</stp>
         <tr r="B29" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3509520532</v>
+        <v>#N/A Requesting Data...3889091718</v>
         <stp/>
         <stp>BDP|12348910938153845212</stp>
         <tr r="B339" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3072057075</v>
+        <v>#N/A Requesting Data...4238731415</v>
         <stp/>
         <stp>BDP|13318321398600849048</stp>
         <tr r="B10" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3909761408</v>
+        <v>#N/A Requesting Data...3647830032</v>
         <stp/>
         <stp>BDP|18435630892228454643</stp>
         <tr r="B394" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3905882763</v>
+        <v>#N/A Requesting Data...4119699682</v>
         <stp/>
         <stp>BDP|17139338150211606906</stp>
         <tr r="B152" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3846334707</v>
+        <v>#N/A Requesting Data...4270975372</v>
         <stp/>
         <stp>BDP|10971712726625894926</stp>
         <tr r="B357" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3157998818</v>
+        <v>#N/A Requesting Data...3862402703</v>
         <stp/>
         <stp>BDP|14695313379829585722</stp>
         <tr r="B217" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3011724700</v>
+        <v>#N/A Requesting Data...3507540808</v>
         <stp/>
         <stp>BDP|17781786592501295670</stp>
         <tr r="B81" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3309437076</v>
+        <v>#N/A Requesting Data...4225882958</v>
         <stp/>
         <stp>BDP|15556548327439527597</stp>
         <tr r="B379" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3291150625</v>
+        <v>#N/A Requesting Data...3841098379</v>
         <stp/>
         <stp>BDP|11127408516558853225</stp>
         <tr r="B202" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3200540137</v>
+        <v>#N/A Requesting Data...3766816887</v>
         <stp/>
         <stp>BDP|12283974065567149401</stp>
         <tr r="B329" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3809063032</v>
+        <v>#N/A Requesting Data...4117208027</v>
         <stp/>
         <stp>BDP|10848356599364479007</stp>
         <tr r="B85" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3393571407</v>
+        <v>#N/A Requesting Data...3629830746</v>
         <stp/>
         <stp>BDP|15469654614484035855</stp>
         <tr r="B108" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3231093608</v>
+        <v>#N/A Requesting Data...4294031539</v>
         <stp/>
         <stp>BDP|14308948137799158937</stp>
         <tr r="B337" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4165346606</v>
+        <v>#N/A Requesting Data...3730295524</v>
         <stp/>
         <stp>BDP|17065062680058010949</stp>
         <tr r="B50" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3456697746</v>
+        <v>#N/A Requesting Data...4056037030</v>
         <stp/>
         <stp>BDP|13009958661901567330</stp>
         <tr r="B270" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4085447012</v>
+        <v>#N/A Requesting Data...4276833940</v>
         <stp/>
         <stp>BDP|10996913360931847078</stp>
         <tr r="B387" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3685805068</v>
+        <v>#N/A Requesting Data...4113682754</v>
         <stp/>
         <stp>BDP|16824325542046324804</stp>
         <tr r="B324" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3921497788</v>
+        <v>#N/A Requesting Data...4219525994</v>
         <stp/>
         <stp>BDP|14699078786662424191</stp>
         <tr r="B75" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3153771876</v>
+        <v>#N/A Requesting Data...3894156911</v>
         <stp/>
         <stp>BDP|13633648184103131189</stp>
         <tr r="B97" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3037240706</v>
+        <v>#N/A Requesting Data...3583940121</v>
         <stp/>
         <stp>BDP|15414268593210618196</stp>
         <tr r="B21" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3058993798</v>
+        <v>#N/A Requesting Data...3740694431</v>
         <stp/>
         <stp>BDP|11175380970389401338</stp>
         <tr r="B200" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3501723262</v>
+        <v>#N/A Requesting Data...3982595782</v>
         <stp/>
         <stp>BDP|12753631390866111442</stp>
         <tr r="B89" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3626224792</v>
+        <v>#N/A Requesting Data...3610048158</v>
         <stp/>
         <stp>BDP|13456853912744487167</stp>
         <tr r="B345" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3989400133</v>
+        <v>#N/A Requesting Data...3780483466</v>
         <stp/>
         <stp>BDP|11021157186101627641</stp>
         <tr r="B292" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3471226064</v>
+        <v>#N/A Requesting Data...3923271351</v>
         <stp/>
         <stp>BDP|10242771696620246137</stp>
         <tr r="B156" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4231312905</v>
+        <v>#N/A Requesting Data...4081833271</v>
         <stp/>
         <stp>BDP|17699790583390064797</stp>
         <tr r="B331" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3035689310</v>
+        <v>#N/A Requesting Data...4292918520</v>
         <stp/>
         <stp>BDP|16945960259977327213</stp>
         <tr r="B229" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3914256779</v>
+        <v>#N/A Requesting Data...3693696119</v>
         <stp/>
         <stp>BDP|18345479815965138747</stp>
         <tr r="B51" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3603639505</v>
+        <v>#N/A Requesting Data...4255267698</v>
         <stp/>
         <stp>BDP|13999808556682163066</stp>
         <tr r="B122" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4145268285</v>
+        <v>#N/A Requesting Data...3602153500</v>
         <stp/>
         <stp>BDP|13812557331681367847</stp>
         <tr r="B251" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3464383945</v>
+        <v>#N/A Requesting Data...4101637636</v>
         <stp/>
         <stp>BDP|12849562285472739177</stp>
         <tr r="B68" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3278470023</v>
+        <v>#N/A Requesting Data...3777907550</v>
         <stp/>
         <stp>BDP|14966066030373580843</stp>
         <tr r="B34" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3718270782</v>
+        <v>#N/A Requesting Data...3980348138</v>
         <stp/>
         <stp>BDP|11761070810659459557</stp>
         <tr r="B31" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4292597399</v>
+        <v>#N/A Requesting Data...4111802270</v>
         <stp/>
         <stp>BDP|11551504287786299603</stp>
         <tr r="B125" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4034850274</v>
+        <v>#N/A Requesting Data...3846738183</v>
         <stp/>
         <stp>BDP|16448970532503096323</stp>
         <tr r="B370" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3562265988</v>
+        <v>#N/A Requesting Data...4149793028</v>
         <stp/>
         <stp>BDP|12525633025602976898</stp>
         <tr r="B392" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3654642036</v>
+        <v>#N/A Requesting Data...3691133138</v>
         <stp/>
         <stp>BDP|17580574377278683149</stp>
         <tr r="B206" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3095310325</v>
+        <v>#N/A Requesting Data...4003986165</v>
         <stp/>
         <stp>BDP|12796095093575392291</stp>
         <tr r="B9" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3645734578</v>
+        <v>#N/A Requesting Data...3814763918</v>
         <stp/>
         <stp>BDP|11473387197264005268</stp>
         <tr r="B208" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4048104738</v>
+        <v>#N/A Requesting Data...3567689225</v>
         <stp/>
         <stp>BDP|10689193314088353556</stp>
         <tr r="B115" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3949960427</v>
+        <v>#N/A Requesting Data...4260455530</v>
         <stp/>
         <stp>BDP|14936255710883418945</stp>
         <tr r="B110" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3567726206</v>
+        <v>#N/A Requesting Data...4226489461</v>
         <stp/>
         <stp>BDP|16436353585357044782</stp>
         <tr r="B185" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4272662122</v>
+        <v>#N/A Requesting Data...4275055903</v>
         <stp/>
         <stp>BDP|17474466698827385065</stp>
         <tr r="B255" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4118424595</v>
+        <v>#N/A Requesting Data...3787611994</v>
         <stp/>
         <stp>BDP|13008978528461747465</stp>
         <tr r="B14" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4177652885</v>
+        <v>#N/A Requesting Data...3738317462</v>
         <stp/>
         <stp>BDP|12963801867899379890</stp>
         <tr r="B42" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3512349617</v>
+        <v>#N/A Requesting Data...4241636998</v>
         <stp/>
         <stp>BDP|14672943994960646944</stp>
         <tr r="B354" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3300010431</v>
+        <v>#N/A Requesting Data...4201303693</v>
         <stp/>
         <stp>BDP|13254853126843011888</stp>
         <tr r="B24" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3178827060</v>
+        <v>#N/A Requesting Data...3736480121</v>
         <stp/>
         <stp>BDP|10833465430244789112</stp>
         <tr r="B138" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3297291636</v>
+        <v>#N/A Requesting Data...3989775387</v>
         <stp/>
         <stp>BDP|12843528775687100535</stp>
         <tr r="B384" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3677717823</v>
+        <v>#N/A Requesting Data...3606920374</v>
         <stp/>
         <stp>BDP|17780737315434401787</stp>
         <tr r="B8" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3955012287</v>
+        <v>#N/A Requesting Data...3820166500</v>
         <stp/>
         <stp>BDP|12002889990921386053</stp>
         <tr r="B196" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3257113254</v>
+        <v>#N/A Requesting Data...4217678618</v>
         <stp/>
         <stp>BDP|10098016291028407342</stp>
         <tr r="B323" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3989372556</v>
+        <v>#N/A Requesting Data...3636657976</v>
         <stp/>
         <stp>BDP|16363745073943149771</stp>
         <tr r="B48" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3722803772</v>
+        <v>#N/A Requesting Data...3821614517</v>
         <stp/>
         <stp>BDP|14799700172311291752</stp>
         <tr r="B87" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3229042091</v>
+        <v>#N/A Requesting Data...4233153491</v>
         <stp/>
         <stp>BDP|10158605034561494646</stp>
         <tr r="B201" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294226198</v>
+        <v>#N/A Requesting Data...3736047631</v>
         <stp/>
         <stp>BDP|10018017332576750708</stp>
         <tr r="B69" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4212500868</v>
+        <v>#N/A Requesting Data...3979829029</v>
         <stp/>
         <stp>BDP|11385042504630044352</stp>
         <tr r="B260" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3388613039</v>
+        <v>#N/A Requesting Data...3914557083</v>
         <stp/>
         <stp>BDP|13915974090327097775</stp>
         <tr r="B257" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3257064212</v>
+        <v>#N/A Requesting Data...3667723014</v>
         <stp/>
         <stp>BDP|14443838958823486906</stp>
         <tr r="B342" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3960083599</v>
+        <v>#N/A Requesting Data...3996499024</v>
         <stp/>
         <stp>BDP|16946029217483762771</stp>
         <tr r="B144" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4007768522</v>
+        <v>#N/A Requesting Data...4018471202</v>
         <stp/>
         <stp>BDP|15156198491527172968</stp>
         <tr r="B36" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3382088425</v>
+        <v>#N/A Requesting Data...4243563738</v>
         <stp/>
         <stp>BDP|15684739062343144478</stp>
         <tr r="B263" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3827405108</v>
+        <v>#N/A Requesting Data...3888484870</v>
         <stp/>
         <stp>BDP|13117150803164619502</stp>
         <tr r="B276" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4274979534</v>
+        <v>#N/A Requesting Data...3808591747</v>
         <stp/>
         <stp>BDP|15060426476344219163</stp>
         <tr r="B124" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3496089388</v>
+        <v>#N/A Requesting Data...3947280570</v>
         <stp/>
         <stp>BDP|17734253039752965727</stp>
         <tr r="B111" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3208509224</v>
+        <v>#N/A Requesting Data...3893651655</v>
         <stp/>
         <stp>BDP|16272590609890454056</stp>
         <tr r="B213" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3392925583</v>
+        <v>#N/A Requesting Data...3888322299</v>
         <stp/>
         <stp>BDP|12723902297580523109</stp>
         <tr r="B44" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3609284400</v>
+        <v>#N/A Requesting Data...4119872381</v>
         <stp/>
         <stp>BDP|10699888615183826962</stp>
         <tr r="B186" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3969947164</v>
+        <v>#N/A Requesting Data...3768596335</v>
         <stp/>
         <stp>BDP|15942502730915807562</stp>
         <tr r="B347" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3427591135</v>
+        <v>#N/A Requesting Data...3598853391</v>
         <stp/>
         <stp>BDP|18224062291181671347</stp>
         <tr r="B199" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3710953462</v>
+        <v>#N/A Requesting Data...3979276495</v>
         <stp/>
         <stp>BDP|18395748308068940412</stp>
         <tr r="B365" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3498987900</v>
+        <v>#N/A Requesting Data...4249788887</v>
         <stp/>
         <stp>BDP|13830456424087680275</stp>
         <tr r="B294" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4211750251</v>
+        <v>#N/A Requesting Data...3857390452</v>
         <stp/>
         <stp>BDP|10862427350184961584</stp>
         <tr r="B224" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4114539301</v>
+        <v>#N/A Requesting Data...3735885601</v>
         <stp/>
         <stp>BDP|16196468959153745424</stp>
         <tr r="B307" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4079437390</v>
+        <v>#N/A Requesting Data...4197095756</v>
         <stp/>
         <stp>BDP|17225043055033751187</stp>
         <tr r="B209" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3951169474</v>
+        <v>#N/A Requesting Data...3761951493</v>
         <stp/>
         <stp>BDP|13501353053214534185</stp>
         <tr r="B176" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3805200126</v>
+        <v>#N/A Requesting Data...3796617456</v>
         <stp/>
         <stp>BDP|13084474983376091956</stp>
         <tr r="B326" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3234474685</v>
+        <v>#N/A Requesting Data...3825066077</v>
         <stp/>
         <stp>BDP|13260185229978467871</stp>
         <tr r="B129" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3195331641</v>
+        <v>#N/A Requesting Data...4113026780</v>
         <stp/>
         <stp>BDP|10118733361113382220</stp>
         <tr r="B237" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3999021617</v>
+        <v>#N/A Requesting Data...4041398891</v>
         <stp/>
         <stp>BDP|10364967257054336840</stp>
         <tr r="B72" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3357439759</v>
+        <v>#N/A Requesting Data...3862018949</v>
         <stp/>
         <stp>BDP|14726342429434070036</stp>
         <tr r="B332" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3402733131</v>
+        <v>#N/A Requesting Data...4166777251</v>
         <stp/>
         <stp>BDP|16543963233999217499</stp>
         <tr r="B96" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4012304004</v>
+        <v>#N/A Requesting Data...4279171302</v>
         <stp/>
         <stp>BDP|14225945679603298819</stp>
         <tr r="B175" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4213158822</v>
+        <v>#N/A Requesting Data...4260159069</v>
         <stp/>
         <stp>BDP|13175082915727268424</stp>
         <tr r="B149" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3163393490</v>
+        <v>#N/A Requesting Data...3618700602</v>
         <stp/>
         <stp>BDP|13762611737035636284</stp>
         <tr r="B250" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3403098055</v>
+        <v>#N/A Requesting Data...3595325148</v>
         <stp/>
         <stp>BDP|17017354836313952554</stp>
         <tr r="B364" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3679593890</v>
+        <v>#N/A Requesting Data...3887659850</v>
         <stp/>
         <stp>BDP|14378320524365661135</stp>
         <tr r="B346" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3783985907</v>
+        <v>#N/A Requesting Data...4121877688</v>
         <stp/>
         <stp>BDP|14559563573727857080</stp>
         <tr r="B20" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3237868025</v>
+        <v>#N/A Requesting Data...3982463692</v>
         <stp/>
         <stp>BDP|17332698423956549495</stp>
         <tr r="B397" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4286556288</v>
+        <v>#N/A Requesting Data...3848900211</v>
         <stp/>
         <stp>BDP|16205340666092175047</stp>
         <tr r="B391" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3491769102</v>
+        <v>#N/A Requesting Data...3815323962</v>
         <stp/>
         <stp>BDP|10464876333332021851</stp>
         <tr r="B106" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3763177556</v>
+        <v>#N/A Requesting Data...4172182174</v>
         <stp/>
         <stp>BDP|17370302188368886548</stp>
         <tr r="B114" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3607160182</v>
+        <v>#N/A Requesting Data...3611246227</v>
         <stp/>
         <stp>BDP|16381332537232440285</stp>
         <tr r="B291" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3439063746</v>
+        <v>#N/A Requesting Data...3627833152</v>
         <stp/>
         <stp>BDP|16487196147064246157</stp>
         <tr r="B127" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4226040332</v>
+        <v>#N/A Requesting Data...3829650688</v>
         <stp/>
         <stp>BDP|17427951471776505940</stp>
         <tr r="B169" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4266394876</v>
+        <v>#N/A Requesting Data...4237293873</v>
         <stp/>
         <stp>BDP|14033132378376827216</stp>
         <tr r="B372" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3890606503</v>
+        <v>#N/A Requesting Data...3662005698</v>
         <stp/>
         <stp>BDP|11252912213578118744</stp>
         <tr r="B101" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3508009001</v>
+        <v>#N/A Requesting Data...4030397151</v>
         <stp/>
         <stp>BDP|11520430921528716940</stp>
         <tr r="B37" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4277929030</v>
+        <v>#N/A Requesting Data...3864169667</v>
         <stp/>
         <stp>BDP|17551700252410397326</stp>
         <tr r="B317" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3618972918</v>
+        <v>#N/A Requesting Data...4161410281</v>
         <stp/>
         <stp>BDP|13578416045592250750</stp>
         <tr r="B280" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3939110312</v>
+        <v>#N/A Requesting Data...4084728562</v>
         <stp/>
         <stp>BDP|11770731031013318003</stp>
         <tr r="B279" s="1"/>
       </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3463222248</v>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A Requesting Data...4063681458</v>
         <stp/>
         <stp>BDP|14937954923660477828</stp>
         <tr r="B253" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096664369</v>
+        <v>#N/A Requesting Data...4228851384</v>
         <stp/>
         <stp>BDP|14300411871210963030</stp>
         <tr r="B353" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4184639524</v>
+        <v>#N/A Requesting Data...3844529179</v>
         <stp/>
         <stp>BDP|14872983979755338800</stp>
         <tr r="B295" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3465404058</v>
+        <v>#N/A Requesting Data...3988575952</v>
         <stp/>
         <stp>BDP|15292204797198733188</stp>
         <tr r="B381" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3928959215</v>
+        <v>#N/A Requesting Data...3774610108</v>
         <stp/>
         <stp>BDP|16322146019636419749</stp>
         <tr r="B283" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3769857113</v>
+        <v>#N/A Requesting Data...4189731480</v>
         <stp/>
         <stp>BDP|16482841280737794694</stp>
         <tr r="B375" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3179430761</v>
+        <v>#N/A Requesting Data...4048181243</v>
         <stp/>
         <stp>BDP|15690629195429496445</stp>
         <tr r="B360" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3625597814</v>
+        <v>#N/A Requesting Data...3965930699</v>
         <stp/>
         <stp>BDP|15777481013801595685</stp>
         <tr r="B314" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3471231884</v>
+        <v>#N/A Requesting Data...4193382200</v>
         <stp/>
         <stp>BDP|11645075884419212749</stp>
         <tr r="B312" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3586431984</v>
+        <v>#N/A Requesting Data...3973992843</v>
         <stp/>
         <stp>BDP|16663166652674560157</stp>
         <tr r="B377" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3663647242</v>
+        <v>#N/A Requesting Data...3774642200</v>
         <stp/>
         <stp>BDP|11883541512632919024</stp>
         <tr r="B132" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3486454535</v>
+        <v>#N/A Requesting Data...3831651386</v>
         <stp/>
         <stp>BDP|10571620270860541653</stp>
         <tr r="B297" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240651440</v>
+        <v>#N/A Requesting Data...3610937290</v>
         <stp/>
         <stp>BDP|12164046345398625903</stp>
         <tr r="B22" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3143317315</v>
+        <v>#N/A Requesting Data...4058173376</v>
         <stp/>
         <stp>BDP|14532285906853232107</stp>
         <tr r="B309" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3214069633</v>
+        <v>#N/A Requesting Data...4227641558</v>
         <stp/>
         <stp>BDP|17009722945667921731</stp>
         <tr r="B288" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3396723539</v>
+        <v>#N/A Requesting Data...4084305780</v>
         <stp/>
         <stp>BDP|11056518109741385175</stp>
         <tr r="B17" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3938435447</v>
+        <v>#N/A Requesting Data...4059349153</v>
         <stp/>
         <stp>BDP|14653412125131141721</stp>
         <tr r="B92" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3938207777</v>
+        <v>#N/A Requesting Data...3813424071</v>
         <stp/>
         <stp>BDP|10017254327654358002</stp>
         <tr r="B320" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3429095720</v>
+        <v>#N/A Requesting Data...3856501589</v>
         <stp/>
         <stp>BDP|12104210233571682675</stp>
         <tr r="B90" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3402219687</v>
+        <v>#N/A Requesting Data...4027646049</v>
         <stp/>
         <stp>BDP|18376875020720220635</stp>
         <tr r="B313" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3168264463</v>
+        <v>#N/A Requesting Data...3973863636</v>
         <stp/>
         <stp>BDP|15381646344572083161</stp>
         <tr r="B61" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3441956156</v>
+        <v>#N/A Requesting Data...3805412085</v>
         <stp/>
         <stp>BDP|15710710243414044607</stp>
         <tr r="B212" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3216692204</v>
+        <v>#N/A Requesting Data...3814568867</v>
         <stp/>
         <stp>BDP|10150509610832622239</stp>
         <tr r="B79" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3372180281</v>
+        <v>#N/A Requesting Data...4053800390</v>
         <stp/>
         <stp>BDP|17930071941962837535</stp>
         <tr r="B289" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4024272195</v>
+        <v>#N/A Requesting Data...4054150007</v>
         <stp/>
         <stp>BDP|15475965082644269465</stp>
         <tr r="B284" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3297583177</v>
+        <v>#N/A Requesting Data...3639038495</v>
         <stp/>
         <stp>BDP|17122345043916276235</stp>
         <tr r="B239" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3532452389</v>
+        <v>#N/A Requesting Data...3879817022</v>
         <stp/>
         <stp>BDP|14652088895669595088</stp>
         <tr r="B171" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4167896953</v>
+        <v>#N/A Requesting Data...4227452578</v>
         <stp/>
         <stp>BDP|12048112663810395083</stp>
         <tr r="B93" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4293959795</v>
+        <v>#N/A Requesting Data...4109209502</v>
         <stp/>
         <stp>BDP|16656488207205119209</stp>
         <tr r="B248" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3698694725</v>
+        <v>#N/A Requesting Data...3955801847</v>
         <stp/>
         <stp>BDP|11748985460889244273</stp>
         <tr r="B193" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3198727135</v>
+        <v>#N/A Requesting Data...3849545165</v>
         <stp/>
         <stp>BDP|12812661744945246020</stp>
         <tr r="B40" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4193423029</v>
+        <v>#N/A Requesting Data...3650460587</v>
         <stp/>
         <stp>BDP|15290007545071484590</stp>
         <tr r="B287" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3826705786</v>
+        <v>#N/A Requesting Data...3656537752</v>
         <stp/>
         <stp>BDP|13044687815236312737</stp>
         <tr r="B133" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3352601111</v>
+        <v>#N/A Requesting Data...3933726004</v>
         <stp/>
         <stp>BDP|18039249928579267400</stp>
         <tr r="B160" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3235115302</v>
+        <v>#N/A Requesting Data...3661647849</v>
         <stp/>
         <stp>BDP|14791360289912333856</stp>
         <tr r="B218" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3560643245</v>
+        <v>#N/A Requesting Data...4104289675</v>
         <stp/>
         <stp>BDP|13261454980663795917</stp>
         <tr r="B249" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3956801250</v>
+        <v>#N/A Requesting Data...4059377876</v>
         <stp/>
         <stp>BDP|15164784883956324984</stp>
         <tr r="B207" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4009936219</v>
+        <v>#N/A Requesting Data...3911824337</v>
         <stp/>
         <stp>BDP|16818842693064932675</stp>
         <tr r="B148" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3993647125</v>
+        <v>#N/A Requesting Data...3747042832</v>
         <stp/>
         <stp>BDP|18194485726023815844</stp>
         <tr r="B23" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3466667974</v>
+        <v>#N/A Requesting Data...3871889236</v>
         <stp/>
         <stp>BDP|16514931462189332520</stp>
         <tr r="B396" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3418227805</v>
+        <v>#N/A Requesting Data...3980340842</v>
         <stp/>
         <stp>BDP|10268528103307436739</stp>
         <tr r="B88" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3460577866</v>
+        <v>#N/A Requesting Data...3784802853</v>
         <stp/>
         <stp>BDP|17260646104021340568</stp>
         <tr r="B141" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4259600470</v>
+        <v>#N/A Requesting Data...3672681578</v>
         <stp/>
         <stp>BDP|15622467935280014731</stp>
         <tr r="B159" s="1"/>
@@ -2429,1279 +2431,1281 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4202614462</v>
+        <v>#N/A Requesting Data...3646692935</v>
         <stp/>
         <stp>BDP|2159967508345186272</stp>
         <tr r="B181" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3926329505</v>
+        <v>#N/A Requesting Data...4280412106</v>
         <stp/>
         <stp>BDP|1616488739962770897</stp>
         <tr r="B215" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240122683</v>
+        <v>#N/A Requesting Data...3851263818</v>
         <stp/>
         <stp>BDP|6634212836503806867</stp>
         <tr r="B226" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3569978999</v>
+        <v>#N/A Requesting Data...3922597362</v>
         <stp/>
         <stp>BDP|3386099434745487963</stp>
         <tr r="B84" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3999450773</v>
+        <v>#N/A Requesting Data...4119141904</v>
         <stp/>
         <stp>BDP|4983811761382457401</stp>
         <tr r="B261" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247936863</v>
+        <v>#N/A Requesting Data...4270411533</v>
         <stp/>
         <stp>BDP|2449849754830247340</stp>
         <tr r="B335" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3940727611</v>
+        <v>#N/A Requesting Data...4123611048</v>
         <stp/>
         <stp>BDP|7645055812508759243</stp>
         <tr r="B184" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3219687806</v>
+        <v>#N/A Requesting Data...4025951924</v>
         <stp/>
         <stp>BDP|5410064290543251311</stp>
         <tr r="B64" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3960401482</v>
+        <v>#N/A Requesting Data...3722167116</v>
         <stp/>
         <stp>BDP|6177995933473570395</stp>
         <tr r="B16" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3252411957</v>
+        <v>#N/A Requesting Data...3652594035</v>
         <stp/>
         <stp>BDP|9537593265211387601</stp>
         <tr r="B343" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3507433918</v>
+        <v>#N/A Requesting Data...3757983915</v>
         <stp/>
         <stp>BDP|1167892644606059660</stp>
         <tr r="B366" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4137236062</v>
+        <v>#N/A Requesting Data...3885407659</v>
         <stp/>
         <stp>BDP|5834159997211518108</stp>
         <tr r="B154" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3455578243</v>
+        <v>#N/A Requesting Data...3991669397</v>
         <stp/>
         <stp>BDP|9111910033109816741</stp>
         <tr r="B126" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4149743967</v>
+        <v>#N/A Requesting Data...4051231115</v>
         <stp/>
         <stp>BDP|9269619323991827171</stp>
         <tr r="B300" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4214181099</v>
+        <v>#N/A Requesting Data...4173327321</v>
         <stp/>
         <stp>BDP|4247076007941746885</stp>
         <tr r="B177" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3729820794</v>
+        <v>#N/A Requesting Data...3665223094</v>
         <stp/>
         <stp>BDP|3663878364346066670</stp>
         <tr r="B305" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3318312675</v>
+        <v>#N/A Requesting Data...4081000935</v>
         <stp/>
         <stp>BDP|9003489115833821275</stp>
         <tr r="B368" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4077326721</v>
+        <v>#N/A Requesting Data...4089426683</v>
         <stp/>
         <stp>BDP|8618524934483334014</stp>
         <tr r="B57" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4011744043</v>
+        <v>#N/A Requesting Data...3724616402</v>
         <stp/>
         <stp>BDP|9056146631571180775</stp>
         <tr r="B210" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046471527</v>
+        <v>#N/A Requesting Data...3827656892</v>
         <stp/>
         <stp>BDP|6763950415927477404</stp>
         <tr r="B77" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3396854676</v>
+        <v>#N/A Requesting Data...4065085973</v>
         <stp/>
         <stp>BDP|5478870364736505025</stp>
         <tr r="B47" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4240714505</v>
+        <v>#N/A Requesting Data...3813151804</v>
         <stp/>
         <stp>BDP|8939393170401073019</stp>
         <tr r="B232" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4249092905</v>
+        <v>#N/A Requesting Data...4074300297</v>
         <stp/>
         <stp>BDP|6179770197970242556</stp>
         <tr r="B161" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4294588296</v>
+        <v>#N/A Requesting Data...3692094316</v>
         <stp/>
         <stp>BDP|9113676763091033527</stp>
         <tr r="B120" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4027160518</v>
+        <v>#N/A Requesting Data...3930498218</v>
         <stp/>
         <stp>BDP|6002571984827368143</stp>
         <tr r="B140" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4092670690</v>
+        <v>#N/A Requesting Data...3764541012</v>
         <stp/>
         <stp>BDP|4714911224751991007</stp>
         <tr r="B327" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A N/A</v>
+        <v>#N/A Requesting Data...3833908673</v>
         <stp/>
         <stp>BDP|2310633811188876373</stp>
         <tr r="B398" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3968841269</v>
+        <v>#N/A Requesting Data...3849783206</v>
         <stp/>
         <stp>BDP|7165273385136536596</stp>
         <tr r="B238" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3567555458</v>
+        <v>#N/A Requesting Data...4222272811</v>
         <stp/>
         <stp>BDP|7097425786430347545</stp>
         <tr r="B163" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3526712760</v>
+        <v>#N/A Requesting Data...4202122112</v>
         <stp/>
         <stp>BDP|5042119580562613045</stp>
         <tr r="B310" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3667999958</v>
+        <v>#N/A Requesting Data...4192478825</v>
         <stp/>
         <stp>BDP|2570732023168291143</stp>
         <tr r="B203" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4040402142</v>
+        <v>#N/A Requesting Data...3810283744</v>
         <stp/>
         <stp>BDP|3324208224455678828</stp>
         <tr r="B298" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3996504165</v>
+        <v>#N/A Requesting Data...4205766010</v>
         <stp/>
         <stp>BDP|9751286653258404882</stp>
         <tr r="B223" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4172869807</v>
+        <v>#N/A Requesting Data...4051794055</v>
         <stp/>
         <stp>BDP|7416845201896194719</stp>
         <tr r="B60" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3894390122</v>
+        <v>#N/A Requesting Data...3781786201</v>
         <stp/>
         <stp>BDP|4811058767269221598</stp>
         <tr r="B341" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3425019510</v>
+        <v>#N/A Requesting Data...4039066340</v>
         <stp/>
         <stp>BDP|5249878353492972480</stp>
         <tr r="B286" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3404892786</v>
+        <v>#N/A Requesting Data...3812484672</v>
         <stp/>
         <stp>BDP|1105503784152648046</stp>
         <tr r="B299" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3699338853</v>
+        <v>#N/A Requesting Data...4036942211</v>
         <stp/>
         <stp>BDP|7954395505129861392</stp>
         <tr r="B197" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3655916004</v>
+        <v>#N/A Requesting Data...3836936411</v>
         <stp/>
         <stp>BDP|8882099850044129747</stp>
         <tr r="B350" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3396241627</v>
+        <v>#N/A Requesting Data...3756931972</v>
         <stp/>
         <stp>BDP|8459459549011747654</stp>
         <tr r="B308" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4166776196</v>
+        <v>#N/A Requesting Data...4235570264</v>
         <stp/>
         <stp>BDP|7787612747492268883</stp>
         <tr r="B178" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3411180728</v>
+        <v>#N/A Requesting Data...4180019985</v>
         <stp/>
         <stp>BDP|5929884769951100507</stp>
         <tr r="B233" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3704373736</v>
+        <v>#N/A Requesting Data...3862505103</v>
         <stp/>
         <stp>BDP|1820375980672799776</stp>
         <tr r="B73" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4194822984</v>
+        <v>#N/A Requesting Data...3936985771</v>
         <stp/>
         <stp>BDP|8511014569283633279</stp>
         <tr r="B4" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3251659569</v>
+        <v>#N/A Requesting Data...4209344205</v>
         <stp/>
         <stp>BDP|9556763907158041983</stp>
         <tr r="B78" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3328316972</v>
+        <v>#N/A Requesting Data...3746197666</v>
         <stp/>
         <stp>BDP|8344579733193318265</stp>
         <tr r="B123" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3734748860</v>
+        <v>#N/A Requesting Data...3995729935</v>
         <stp/>
         <stp>BDP|8401903946882489801</stp>
         <tr r="B328" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3878763214</v>
+        <v>#N/A Requesting Data...4183121283</v>
         <stp/>
         <stp>BDP|5566915924510698123</stp>
         <tr r="B192" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3898229131</v>
+        <v>#N/A Requesting Data...4272551687</v>
         <stp/>
         <stp>BDP|1755057291660146099</stp>
         <tr r="B165" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3863363653</v>
+        <v>#N/A Requesting Data...4201547295</v>
         <stp/>
         <stp>BDP|3772879838925471557</stp>
         <tr r="B216" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3967618609</v>
+        <v>#N/A Requesting Data...3880842018</v>
         <stp/>
         <stp>BDP|8067889687407371733</stp>
         <tr r="B361" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3862003486</v>
+        <v>#N/A Requesting Data...4009268140</v>
         <stp/>
         <stp>BDP|9256373552323938439</stp>
         <tr r="B2" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3967375431</v>
+        <v>#N/A Requesting Data...4058587318</v>
         <stp/>
         <stp>BDP|4130271573900859909</stp>
         <tr r="B374" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3935381655</v>
+        <v>#N/A Requesting Data...4290854578</v>
         <stp/>
         <stp>BDP|8441650713235108213</stp>
         <tr r="B318" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3798533933</v>
+        <v>#N/A Requesting Data...4106616340</v>
         <stp/>
         <stp>BDP|5504607586014954786</stp>
         <tr r="B121" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3683906803</v>
+        <v>#N/A Requesting Data...4193595467</v>
         <stp/>
         <stp>BDP|3204982408462384004</stp>
         <tr r="B166" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3847961370</v>
+        <v>#N/A Requesting Data...3708674539</v>
         <stp/>
         <stp>BDP|8437157569272730594</stp>
         <tr r="B18" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3480005488</v>
+        <v>#N/A Requesting Data...4225630355</v>
         <stp/>
         <stp>BDP|7209768445924133864</stp>
         <tr r="B204" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4158548264</v>
+        <v>#N/A Requesting Data...4004442885</v>
         <stp/>
         <stp>BDP|6851387782125480014</stp>
         <tr r="B231" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4255294651</v>
+        <v>#N/A Requesting Data...4195880069</v>
         <stp/>
         <stp>BDP|5452121751471556856</stp>
         <tr r="B389" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3468803948</v>
+        <v>#N/A Requesting Data...3837048193</v>
         <stp/>
         <stp>BDP|6403863836080625553</stp>
         <tr r="B45" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3658657843</v>
+        <v>#N/A Requesting Data...3849303411</v>
         <stp/>
         <stp>BDP|7538464451476053863</stp>
         <tr r="B277" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3763533707</v>
+        <v>#N/A Requesting Data...3810172051</v>
         <stp/>
         <stp>BDP|9013377987228351265</stp>
         <tr r="B158" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3961497813</v>
+        <v>#N/A Requesting Data...4201371507</v>
         <stp/>
         <stp>BDP|4337816978804765672</stp>
         <tr r="B367" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3664416679</v>
+        <v>#N/A Requesting Data...4044122659</v>
         <stp/>
         <stp>BDP|8446436669956060550</stp>
         <tr r="B145" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4223579577</v>
+        <v>#N/A Requesting Data...3708779696</v>
         <stp/>
         <stp>BDP|1587984046253750641</stp>
         <tr r="B119" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4207794978</v>
+        <v>#N/A Requesting Data...3771840523</v>
         <stp/>
         <stp>BDP|1026216078554804983</stp>
         <tr r="B363" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4036131682</v>
+        <v>#N/A Requesting Data...4237800691</v>
         <stp/>
         <stp>BDP|2154178838058624119</stp>
         <tr r="B383" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3511670496</v>
+        <v>#N/A Requesting Data...4237390747</v>
         <stp/>
         <stp>BDP|3756993711195046700</stp>
         <tr r="B334" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3417480118</v>
+        <v>#N/A Requesting Data...3930250363</v>
         <stp/>
         <stp>BDP|1778188670076573885</stp>
         <tr r="B235" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3779868615</v>
+        <v>#N/A Requesting Data...3775923781</v>
         <stp/>
         <stp>BDP|3328558479650879844</stp>
         <tr r="B104" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3324971515</v>
+        <v>#N/A Requesting Data...4264039584</v>
         <stp/>
         <stp>BDP|7387732507119037066</stp>
         <tr r="B293" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3542272072</v>
+        <v>#N/A Requesting Data...3893249272</v>
         <stp/>
         <stp>BDP|6901586044717678928</stp>
         <tr r="B356" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3244047789</v>
+        <v>#N/A Requesting Data...3843714544</v>
         <stp/>
         <stp>BDP|9948588698769440596</stp>
         <tr r="B315" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4210473825</v>
+        <v>#N/A Requesting Data...3919039092</v>
         <stp/>
         <stp>BDP|8306282837618898812</stp>
         <tr r="B105" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3378612208</v>
+        <v>#N/A Requesting Data...4278594526</v>
         <stp/>
         <stp>BDP|4034035877338714188</stp>
         <tr r="B66" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3789820319</v>
+        <v>#N/A Requesting Data...3814539521</v>
         <stp/>
         <stp>BDP|6504982155884336431</stp>
         <tr r="B46" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3577972578</v>
+        <v>#N/A Requesting Data...3907056541</v>
         <stp/>
         <stp>BDP|9539666714016698283</stp>
         <tr r="B230" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3738585541</v>
+        <v>#N/A Requesting Data...3970617007</v>
         <stp/>
         <stp>BDP|5262526435029964023</stp>
         <tr r="B362" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3507084749</v>
+        <v>#N/A Requesting Data...4035707339</v>
         <stp/>
         <stp>BDP|3304744725439832569</stp>
         <tr r="B27" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4285544466</v>
+        <v>#N/A Requesting Data...4026574031</v>
         <stp/>
         <stp>BDP|3255832905984804513</stp>
         <tr r="B103" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3325050007</v>
+        <v>#N/A Requesting Data...4183183797</v>
         <stp/>
         <stp>BDP|5573926401863462510</stp>
         <tr r="B269" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175043158</v>
+        <v>#N/A Requesting Data...3882936520</v>
         <stp/>
         <stp>BDP|4786697258628754514</stp>
         <tr r="B319" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3339773206</v>
+        <v>#N/A Requesting Data...3847434933</v>
         <stp/>
         <stp>BDP|8287211521163460177</stp>
         <tr r="B146" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3281795183</v>
+        <v>#N/A Requesting Data...3785122962</v>
         <stp/>
         <stp>BDP|9086064252601876678</stp>
         <tr r="B234" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3346292996</v>
+        <v>#N/A Requesting Data...4006332768</v>
         <stp/>
         <stp>BDP|9133009717042871168</stp>
         <tr r="B38" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3589459163</v>
+        <v>#N/A Requesting Data...4130812522</v>
         <stp/>
         <stp>BDP|9490247145635802133</stp>
         <tr r="B221" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3890927233</v>
+        <v>#N/A Requesting Data...3954964946</v>
         <stp/>
         <stp>BDP|6125687186584511761</stp>
         <tr r="B153" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3497074013</v>
+        <v>#N/A Requesting Data...4275819860</v>
         <stp/>
         <stp>BDP|2707086532819151308</stp>
         <tr r="B70" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3504624277</v>
+        <v>#N/A Requesting Data...3990900632</v>
         <stp/>
         <stp>BDP|7074656770148625508</stp>
         <tr r="B155" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046295729</v>
+        <v>#N/A Requesting Data...4227248360</v>
         <stp/>
         <stp>BDP|2964127099354269511</stp>
         <tr r="B6" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3440627177</v>
+        <v>#N/A Requesting Data...4173126913</v>
         <stp/>
         <stp>BDP|1956887064617314372</stp>
         <tr r="B259" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3867393241</v>
+        <v>#N/A Requesting Data...3942605796</v>
         <stp/>
         <stp>BDP|3665966951652755600</stp>
         <tr r="B390" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3319888487</v>
+        <v>#N/A Requesting Data...3816004561</v>
         <stp/>
         <stp>BDP|2938319088500630215</stp>
         <tr r="B33" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3948128799</v>
+        <v>#N/A Requesting Data...4094645391</v>
         <stp/>
         <stp>BDP|8654634741431788043</stp>
         <tr r="B338" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3678808340</v>
+        <v>#N/A Requesting Data...4210129936</v>
         <stp/>
         <stp>BDP|4697581877355937852</stp>
         <tr r="B349" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4196376072</v>
+        <v>#N/A Requesting Data...3895382500</v>
         <stp/>
         <stp>BDP|5602901118536251090</stp>
         <tr r="B167" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3300284815</v>
+        <v>#N/A Requesting Data...3748468598</v>
         <stp/>
         <stp>BDP|5723318967577265383</stp>
         <tr r="B137" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4081745628</v>
+        <v>#N/A Requesting Data...4017336566</v>
         <stp/>
         <stp>BDP|5299383097938362365</stp>
         <tr r="B65" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4128885904</v>
+        <v>#N/A Requesting Data...4055295120</v>
         <stp/>
         <stp>BDP|6790830305569666344</stp>
         <tr r="B172" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4015155094</v>
+        <v>#N/A Requesting Data...3806087415</v>
         <stp/>
         <stp>BDP|4450690634380837522</stp>
         <tr r="B242" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4018930235</v>
+        <v>#N/A Requesting Data...4030676989</v>
         <stp/>
         <stp>BDP|9972996890465181803</stp>
         <tr r="B15" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3617283078</v>
+        <v>#N/A Requesting Data...4073682957</v>
         <stp/>
         <stp>BDP|1365832184647286205</stp>
         <tr r="B268" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3690504613</v>
+        <v>#N/A Requesting Data...3985107381</v>
         <stp/>
         <stp>BDP|5964018405295762542</stp>
         <tr r="B28" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3654537615</v>
+        <v>#N/A Requesting Data...3975775190</v>
         <stp/>
         <stp>BDP|7521872191493878056</stp>
         <tr r="B376" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3313312885</v>
+        <v>#N/A Requesting Data...4279273649</v>
         <stp/>
         <stp>BDP|6007357114167846665</stp>
         <tr r="B142" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3877397713</v>
+        <v>#N/A Requesting Data...4095431821</v>
         <stp/>
         <stp>BDP|7502777392035983955</stp>
         <tr r="B191" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4191525009</v>
+        <v>#N/A Requesting Data...3763446600</v>
         <stp/>
         <stp>BDP|1639738779737179316</stp>
         <tr r="B82" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3682961389</v>
+        <v>#N/A Requesting Data...3831008345</v>
         <stp/>
         <stp>BDP|2120703905663159382</stp>
         <tr r="B174" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4098445442</v>
+        <v>#N/A Requesting Data...4146915833</v>
         <stp/>
         <stp>BDP|6742385302118835878</stp>
         <tr r="B330" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4228542914</v>
+        <v>#N/A Requesting Data...3811851190</v>
         <stp/>
         <stp>BDP|4360128176313246459</stp>
         <tr r="B256" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3906820534</v>
+        <v>#N/A Requesting Data...3921294564</v>
         <stp/>
         <stp>BDP|8766224565429045016</stp>
         <tr r="B285" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4169981626</v>
+        <v>#N/A Requesting Data...4102196854</v>
         <stp/>
         <stp>BDP|4302103893728209146</stp>
         <tr r="B282" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3505885744</v>
+        <v>#N/A Requesting Data...3822893364</v>
         <stp/>
         <stp>BDP|2525768650556155370</stp>
         <tr r="B301" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3653270040</v>
+        <v>#N/A Requesting Data...3822488666</v>
         <stp/>
         <stp>BDP|7480052038699543896</stp>
         <tr r="B369" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4075986222</v>
+        <v>#N/A Requesting Data...4167069148</v>
         <stp/>
         <stp>BDP|6809137966025255257</stp>
         <tr r="B173" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3783891126</v>
+        <v>#N/A Requesting Data...3981542052</v>
         <stp/>
         <stp>BDP|3167785075055714025</stp>
         <tr r="B157" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4006955812</v>
+        <v>#N/A Requesting Data...3942195644</v>
         <stp/>
         <stp>BDP|2497194249297948636</stp>
         <tr r="B25" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3364339498</v>
+        <v>#N/A Requesting Data...3777654560</v>
         <stp/>
         <stp>BDP|9439413699257628547</stp>
         <tr r="B3" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046006343</v>
+        <v>#N/A Requesting Data...3891208604</v>
         <stp/>
         <stp>BDP|8454449977289088488</stp>
         <tr r="B117" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4164526881</v>
+        <v>#N/A Requesting Data...3885794225</v>
         <stp/>
         <stp>BDP|1803010743823299042</stp>
         <tr r="B311" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3664574887</v>
+        <v>#N/A Requesting Data...4073114505</v>
         <stp/>
         <stp>BDP|3653227407547923084</stp>
         <tr r="B49" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3850200542</v>
+        <v>#N/A Requesting Data...3801568348</v>
         <stp/>
         <stp>BDP|2756890649150563811</stp>
         <tr r="B355" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3499579508</v>
+        <v>#N/A Requesting Data...4240092356</v>
         <stp/>
         <stp>BDP|7324120960201532749</stp>
         <tr r="B130" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3930842231</v>
+        <v>#N/A Requesting Data...3800894919</v>
         <stp/>
         <stp>BDP|1067302361210244220</stp>
         <tr r="B211" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3965854344</v>
+        <v>#N/A Requesting Data...4091322499</v>
         <stp/>
         <stp>BDP|5908412448375668604</stp>
         <tr r="B54" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4028440283</v>
+        <v>#N/A Requesting Data...3880210925</v>
         <stp/>
         <stp>BDP|4392521002186387158</stp>
         <tr r="B136" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3918921259</v>
+        <v>#N/A Requesting Data...4224357664</v>
         <stp/>
         <stp>BDP|8012676081359136929</stp>
         <tr r="B74" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3545927196</v>
+        <v>#N/A Requesting Data...3942529265</v>
         <stp/>
         <stp>BDP|4026237179456813081</stp>
         <tr r="B386" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3848804510</v>
+        <v>#N/A Requesting Data...4121633531</v>
         <stp/>
         <stp>BDP|6695492446228728949</stp>
         <tr r="B39" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3722011160</v>
+        <v>#N/A Requesting Data...4164815804</v>
         <stp/>
         <stp>BDP|7872241775991604465</stp>
         <tr r="B134" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3686312139</v>
+        <v>#N/A Requesting Data...4010165865</v>
         <stp/>
         <stp>BDP|4084823897225339785</stp>
         <tr r="B13" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4166461452</v>
+        <v>#N/A Requesting Data...4180284709</v>
         <stp/>
         <stp>BDP|1934556223780562144</stp>
         <tr r="B194" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3955353345</v>
+        <v>#N/A Requesting Data...3896192240</v>
         <stp/>
         <stp>BDP|8048315437187166890</stp>
         <tr r="B102" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4006018390</v>
+        <v>#N/A Requesting Data...3906044994</v>
         <stp/>
         <stp>BDP|4278213735880902207</stp>
         <tr r="B303" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3366639499</v>
+        <v>#N/A Requesting Data...3998650354</v>
         <stp/>
         <stp>BDP|8784148998690980761</stp>
         <tr r="B94" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3962631720</v>
+        <v>#N/A Requesting Data...3919632809</v>
         <stp/>
         <stp>BDP|9284429991567405417</stp>
         <tr r="B71" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3658969240</v>
+        <v>#N/A Requesting Data...4030579620</v>
         <stp/>
         <stp>BDP|3675933788074191196</stp>
         <tr r="B275" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3960265333</v>
+        <v>#N/A Requesting Data...3828314250</v>
         <stp/>
         <stp>BDP|7971603600064916587</stp>
         <tr r="B258" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3552674231</v>
+        <v>#N/A Requesting Data...4118860234</v>
         <stp/>
         <stp>BDP|6757851439784119920</stp>
         <tr r="B225" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3470924427</v>
+        <v>#N/A Requesting Data...3824387303</v>
         <stp/>
         <stp>BDP|7087797093831456811</stp>
         <tr r="B139" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3425331914</v>
+        <v>#N/A Requesting Data...3872402015</v>
         <stp/>
         <stp>BDP|2190043708232173005</stp>
         <tr r="B240" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3483385810</v>
+        <v>#N/A Requesting Data...3949127223</v>
         <stp/>
         <stp>BDP|2707611907293501781</stp>
         <tr r="B304" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3714758510</v>
+        <v>#N/A Requesting Data...3893715647</v>
         <stp/>
         <stp>BDP|5383506011184981597</stp>
         <tr r="B86" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4037276650</v>
+        <v>#N/A Requesting Data...4148189887</v>
         <stp/>
         <stp>BDP|7325759456636415359</stp>
         <tr r="B183" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4236538667</v>
+        <v>#N/A Requesting Data...3949608531</v>
         <stp/>
         <stp>BDP|6529624563456338016</stp>
         <tr r="B393" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3763589458</v>
+        <v>#N/A Requesting Data...4193637228</v>
         <stp/>
         <stp>BDP|8737782139495759949</stp>
         <tr r="B168" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4102542267</v>
+        <v>#N/A Requesting Data...4180785291</v>
         <stp/>
         <stp>BDP|5014005604456065313</stp>
         <tr r="B296" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4109792115</v>
+        <v>#N/A Requesting Data...3801275203</v>
         <stp/>
         <stp>BDP|5272023246400067130</stp>
         <tr r="B99" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3453191183</v>
+        <v>#N/A Requesting Data...4195956242</v>
         <stp/>
         <stp>BDP|1671551152586386685</stp>
         <tr r="B322" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3624142577</v>
+        <v>#N/A Requesting Data...4083454223</v>
         <stp/>
         <stp>BDP|6142732972860358785</stp>
         <tr r="B19" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3551575776</v>
+        <v>#N/A Requesting Data...3973376721</v>
         <stp/>
         <stp>BDP|2542458366896861750</stp>
         <tr r="B267" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4125443257</v>
+        <v>#N/A Requesting Data...3843111671</v>
         <stp/>
         <stp>BDP|3251320817148613896</stp>
         <tr r="B378" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3521522540</v>
+        <v>#N/A Requesting Data...3912940761</v>
         <stp/>
         <stp>BDP|1690586617594287034</stp>
         <tr r="B62" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3459002953</v>
+        <v>#N/A Requesting Data...4034352204</v>
         <stp/>
         <stp>BDP|5137403842162895626</stp>
         <tr r="B189" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3747652680</v>
+        <v>#N/A Requesting Data...4124386189</v>
         <stp/>
         <stp>BDP|2660667301590727589</stp>
         <tr r="B243" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3943356817</v>
+        <v>#N/A Requesting Data...3929527773</v>
         <stp/>
         <stp>BDP|3073691645510503065</stp>
         <tr r="B83" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4247884089</v>
+        <v>#N/A Requesting Data...4238157352</v>
         <stp/>
         <stp>BDP|5933370867924533508</stp>
         <tr r="B247" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3404254210</v>
+        <v>#N/A Requesting Data...4226379647</v>
         <stp/>
         <stp>BDP|5093934790545830166</stp>
         <tr r="B214" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3559894397</v>
+        <v>#N/A Requesting Data...4082238171</v>
         <stp/>
         <stp>BDP|1573135905830272139</stp>
         <tr r="B55" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4094673409</v>
+        <v>#N/A Requesting Data...4211580859</v>
         <stp/>
         <stp>BDP|4869270792746604883</stp>
         <tr r="B325" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3993898000</v>
+        <v>#N/A Requesting Data...3963276679</v>
         <stp/>
         <stp>BDP|9067920579062203497</stp>
         <tr r="B371" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3877285996</v>
+        <v>#N/A Requesting Data...4198460614</v>
         <stp/>
         <stp>BDP|6694148016020184731</stp>
         <tr r="B271" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4060238242</v>
+        <v>#N/A Requesting Data...4124709399</v>
         <stp/>
         <stp>BDP|8287501159908428182</stp>
         <tr r="B274" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3382844815</v>
+        <v>#N/A Requesting Data...4109749533</v>
         <stp/>
         <stp>BDP|9566681757602920978</stp>
         <tr r="B340" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3369900334</v>
+        <v>#N/A Requesting Data...4039024060</v>
         <stp/>
         <stp>BDP|1251668447084914524</stp>
         <tr r="B220" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3609664031</v>
+        <v>#N/A Requesting Data...4083938749</v>
         <stp/>
         <stp>BDP|4026696791999045016</stp>
         <tr r="B80" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3696530400</v>
+        <v>#N/A Requesting Data...3956287489</v>
         <stp/>
         <stp>BDP|4773820777991352888</stp>
         <tr r="B344" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3697368884</v>
+        <v>#N/A Requesting Data...4138678752</v>
         <stp/>
         <stp>BDP|6983505214603321306</stp>
         <tr r="B252" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3713373708</v>
+        <v>#N/A Requesting Data...3936552346</v>
         <stp/>
         <stp>BDP|4362063935462802761</stp>
         <tr r="B333" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3519870873</v>
+        <v>#N/A Requesting Data...4169335687</v>
         <stp/>
         <stp>BDP|2075099440401407511</stp>
         <tr r="B205" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3692848482</v>
+        <v>#N/A Requesting Data...3948265210</v>
         <stp/>
         <stp>BDP|3599497292185539972</stp>
         <tr r="B95" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3452243076</v>
+        <v>#N/A Requesting Data...3848205133</v>
         <stp/>
         <stp>BDP|5882781668123225595</stp>
         <tr r="B109" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3812144706</v>
+        <v>#N/A Requesting Data...3981372581</v>
         <stp/>
         <stp>BDP|2690403022986727051</stp>
         <tr r="B306" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4228428603</v>
+        <v>#N/A Requesting Data...4283013945</v>
         <stp/>
         <stp>BDP|2914254001613272189</stp>
         <tr r="B254" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4028563995</v>
+        <v>#N/A Requesting Data...4257015815</v>
         <stp/>
         <stp>BDP|7791838532636213837</stp>
         <tr r="B190" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4062401522</v>
+        <v>#N/A Requesting Data...3939194859</v>
         <stp/>
         <stp>BDP|3138450948746022785</stp>
         <tr r="B388" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3606752412</v>
+        <v>#N/A Requesting Data...4196368068</v>
         <stp/>
         <stp>BDP|8297765501229589458</stp>
         <tr r="B100" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3977971687</v>
+        <v>#N/A Requesting Data...4035315127</v>
         <stp/>
         <stp>BDP|6444891752269511118</stp>
         <tr r="B98" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4133738068</v>
+        <v>#N/A Requesting Data...3876440107</v>
         <stp/>
         <stp>BDP|8831739080485089101</stp>
         <tr r="B128" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3899221326</v>
+        <v>#N/A Requesting Data...3926175391</v>
         <stp/>
         <stp>BDP|3936089777827836074</stp>
         <tr r="B281" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3345783275</v>
+        <v>#N/A Requesting Data...4002822876</v>
         <stp/>
         <stp>BDP|7624206463972900232</stp>
         <tr r="B43" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3764684883</v>
+        <v>#N/A Requesting Data...4025044289</v>
         <stp/>
         <stp>BDP|4518281413433415757</stp>
         <tr r="B395" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3960453866</v>
+        <v>#N/A Requesting Data...4207809067</v>
         <stp/>
         <stp>BDP|3976096571603930445</stp>
         <tr r="B262" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4157713408</v>
+        <v>#N/A Requesting Data...4291644730</v>
         <stp/>
         <stp>BDP|6215528914530076161</stp>
         <tr r="B264" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4291469731</v>
+        <v>#N/A Requesting Data...4000204636</v>
         <stp/>
         <stp>BDP|4352979402866174852</stp>
         <tr r="B135" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4030428729</v>
+        <v>#N/A Requesting Data...3916837027</v>
         <stp/>
         <stp>BDP|5886522167892769784</stp>
         <tr r="B162" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3897140185</v>
+        <v>#N/A Requesting Data...4169974918</v>
         <stp/>
         <stp>BDP|2677410925874398367</stp>
         <tr r="B67" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3742556618</v>
+        <v>#N/A Requesting Data...4183521777</v>
         <stp/>
         <stp>BDP|9203006611463391879</stp>
         <tr r="B266" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3598271391</v>
+        <v>#N/A Requesting Data...3927091072</v>
         <stp/>
         <stp>BDP|1837482273976713702</stp>
         <tr r="B244" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3587337846</v>
+        <v>#N/A Requesting Data...3943240347</v>
         <stp/>
         <stp>BDP|1146746445751790036</stp>
         <tr r="B11" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3373202286</v>
+        <v>#N/A Requesting Data...4040719300</v>
         <stp/>
         <stp>BDP|5021634321890294245</stp>
         <tr r="B131" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4288548995</v>
+        <v>#N/A Requesting Data...4281236828</v>
         <stp/>
         <stp>BDP|3081084245004109092</stp>
         <tr r="B151" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4133067772</v>
+        <v>#N/A Requesting Data...4008813397</v>
         <stp/>
         <stp>BDP|8196645112258459465</stp>
         <tr r="B278" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4135681496</v>
+        <v>#N/A Requesting Data...4120179688</v>
         <stp/>
         <stp>BDP|83225485869737838</stp>
         <tr r="B359" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3525361414</v>
+        <v>#N/A Requesting Data...3877295397</v>
         <stp/>
         <stp>BDP|70005085942109733</stp>
         <tr r="B382" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3545130592</v>
+        <v>#N/A Requesting Data...3923360790</v>
         <stp/>
         <stp>BDP|14363976206455558</stp>
         <tr r="B56" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3740318092</v>
+        <v>#N/A Requesting Data...3945796793</v>
         <stp/>
         <stp>BDP|84106375613917378</stp>
         <tr r="B302" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3381404108</v>
+        <v>#N/A Requesting Data...3979220578</v>
         <stp/>
         <stp>BDP|655303338382162756</stp>
         <tr r="B107" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3386667720</v>
+        <v>#N/A Requesting Data...4085516120</v>
         <stp/>
         <stp>BDP|749570913491215057</stp>
         <tr r="B222" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4109040567</v>
+        <v>#N/A Requesting Data...4195753141</v>
         <stp/>
         <stp>BDP|602854865312240813</stp>
         <tr r="B227" s="1"/>
       </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4149957234</v>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A Requesting Data...4147790410</v>
         <stp/>
         <stp>BDP|852790523643810016</stp>
         <tr r="B219" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4221432660</v>
+        <v>#N/A Requesting Data...4270776809</v>
         <stp/>
         <stp>BDP|110725622775637199</stp>
         <tr r="B321" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3908366691</v>
+        <v>#N/A Requesting Data...3985350072</v>
         <stp/>
         <stp>BDP|842225605347875488</stp>
         <tr r="B113" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4248311964</v>
+        <v>#N/A Requesting Data...4136105523</v>
         <stp/>
         <stp>BDP|487028466072771555</stp>
         <tr r="B59" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="b">
+        <v>0</v>
         <stp/>
         <stp>BSRCH|15411063609594630250</stp>
         <tr r="A1" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3780075268</v>
+        <v>#N/A Requesting Data...3909546012</v>
         <stp/>
         <stp>BDP|140625555810630171</stp>
         <tr r="B118" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4210691725</v>
+        <v>#N/A Requesting Data...4180139982</v>
         <stp/>
         <stp>BDP|774478735417763200</stp>
         <tr r="B116" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4121607317</v>
+        <v>#N/A Requesting Data...4290686526</v>
         <stp/>
         <stp>BDP|800566262909001729</stp>
         <tr r="B236" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3653092651</v>
+        <v>#N/A Requesting Data...3995759142</v>
         <stp/>
         <stp>BDP|888798819428549328</stp>
         <tr r="B351" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3455017566</v>
+        <v>#N/A Requesting Data...3995538941</v>
         <stp/>
         <stp>BDP|585949805455044028</stp>
         <tr r="B35" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3943544545</v>
+        <v>#N/A Requesting Data...4231388998</v>
         <stp/>
         <stp>BDP|967016015949489229</stp>
         <tr r="B30" s="1"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3958996816</v>
+        <v>#N/A Requesting Data...4155227523</v>
         <stp/>
         <stp>BDP|849343358779752513</stp>
         <tr r="B7" s="1"/>
@@ -4030,8 +4034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15CAB35-8BE7-4773-B887-2FBAD6D5E20C}">
   <dimension ref="A1:H398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="R342" sqref="R342"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="L375" sqref="L375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>